<commit_message>
commit change conftest and xlsx file
</commit_message>
<xml_diff>
--- a/Testdata/logintestdata.xlsx
+++ b/Testdata/logintestdata.xlsx
@@ -39,19 +39,19 @@
     <t>Fail</t>
   </si>
   <si>
-    <t>adm@yourstore.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">admin </t>
   </si>
   <si>
     <t>adm</t>
   </si>
   <si>
-    <t>adm@youstore.com</t>
-  </si>
-  <si>
     <t>admin@yourstore.com</t>
+  </si>
+  <si>
+    <t>admincase3@yourstore.com</t>
+  </si>
+  <si>
+    <t>admincase4@yourstore.com</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -456,7 +456,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -470,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -478,10 +478,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
@@ -489,10 +489,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>

</xml_diff>